<commit_message>
chore: Update tasks tracking spreadsheet with completed items
Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/tasks_updated.xlsx
+++ b/tasks_updated.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="285">
   <si>
     <t>כותרת</t>
   </si>
@@ -808,15 +808,18 @@
     <t>⏳ לבדיקה - תלוי בbackend</t>
   </si>
   <si>
+    <t>✅ בוצע - החיפוש כבר ריאקטיבי עם debounce</t>
+  </si>
+  <si>
+    <t>✅ בוצע - כבר קיים בSubmitExpense</t>
+  </si>
+  <si>
+    <t>✅ בוצע - אין כפילות בקוד</t>
+  </si>
+  <si>
     <t>⏳ לבדיקה</t>
   </si>
   <si>
-    <t>✅ בוצע - כבר קיים בSubmitExpense</t>
-  </si>
-  <si>
-    <t>✅ בוצע - אין כפילות בקוד</t>
-  </si>
-  <si>
     <t>✅ בוצע - כבר קיים בDepartmentManager</t>
   </si>
   <si>
@@ -841,19 +844,31 @@
     <t>✅ בוצע - TomSelectInput בעריכה</t>
   </si>
   <si>
+    <t>✅ בוצע - נוסף debounce לפילטרים</t>
+  </si>
+  <si>
     <t>✅ בוצע - כותרת sticky</t>
   </si>
   <si>
     <t>✅ בוצע - reset של input value</t>
   </si>
   <si>
+    <t>✅ בוצע - נוסף debounce + allowClear לדרופדאונים</t>
+  </si>
+  <si>
     <t>✅ בוצע - Payment Due מותנה בbank_transfer</t>
   </si>
   <si>
     <t>✅ בוצע - לחיצה על שורה פותחת פרטים</t>
   </si>
   <si>
+    <t>✅ בוצע - כבר קיים TomSelect עם createNewOption</t>
+  </si>
+  <si>
     <t>✅ בוצע - הוחלף Cash ב-Standing Order</t>
+  </si>
+  <si>
+    <t>✅ בוצע - נוסף דרופדאון שנת תקציב עם אזהרה בעת שינוי</t>
   </si>
 </sst>
 </file>
@@ -1542,7 +1557,7 @@
         <v>254</v>
       </c>
       <c r="J11" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -1600,7 +1615,7 @@
         <v>244</v>
       </c>
       <c r="J13" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -1629,7 +1644,7 @@
         <v>245</v>
       </c>
       <c r="J14" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -1658,7 +1673,7 @@
         <v>246</v>
       </c>
       <c r="J15" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -1687,7 +1702,7 @@
         <v>247</v>
       </c>
       <c r="J16" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -1716,7 +1731,7 @@
         <v>245</v>
       </c>
       <c r="J17" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -1774,7 +1789,7 @@
         <v>240</v>
       </c>
       <c r="J19" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -1803,7 +1818,7 @@
         <v>235</v>
       </c>
       <c r="J20" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -1832,7 +1847,7 @@
         <v>248</v>
       </c>
       <c r="J21" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -1861,7 +1876,7 @@
         <v>249</v>
       </c>
       <c r="J22" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -1919,7 +1934,7 @@
         <v>249</v>
       </c>
       <c r="J24" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -2012,7 +2027,7 @@
         <v>256</v>
       </c>
       <c r="J27" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -2041,7 +2056,7 @@
         <v>235</v>
       </c>
       <c r="J28" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -2070,7 +2085,7 @@
         <v>249</v>
       </c>
       <c r="J29" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -2099,7 +2114,7 @@
         <v>250</v>
       </c>
       <c r="J30" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -2157,7 +2172,7 @@
         <v>250</v>
       </c>
       <c r="J32" t="s">
-        <v>264</v>
+        <v>276</v>
       </c>
     </row>
     <row r="33" spans="1:10">
@@ -2189,7 +2204,7 @@
         <v>257</v>
       </c>
       <c r="J33" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
     </row>
     <row r="34" spans="1:10">
@@ -2250,7 +2265,7 @@
         <v>250</v>
       </c>
       <c r="J35" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
     </row>
     <row r="36" spans="1:10">
@@ -2337,7 +2352,7 @@
         <v>235</v>
       </c>
       <c r="J38" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
     </row>
     <row r="39" spans="1:10">
@@ -2366,7 +2381,7 @@
         <v>240</v>
       </c>
       <c r="J39" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
     </row>
     <row r="40" spans="1:10">
@@ -2395,7 +2410,7 @@
         <v>235</v>
       </c>
       <c r="J40" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
     </row>
     <row r="41" spans="1:10">
@@ -2424,7 +2439,7 @@
         <v>250</v>
       </c>
       <c r="J41" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
     </row>
     <row r="42" spans="1:10">
@@ -2453,7 +2468,7 @@
         <v>250</v>
       </c>
       <c r="J42" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
     </row>
     <row r="43" spans="1:10">
@@ -2511,7 +2526,7 @@
         <v>250</v>
       </c>
       <c r="J44" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
     </row>
     <row r="45" spans="1:10">
@@ -2540,7 +2555,7 @@
         <v>235</v>
       </c>
       <c r="J45" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
     </row>
     <row r="46" spans="1:10">
@@ -2548,7 +2563,7 @@
         <v>54</v>
       </c>
       <c r="J46" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
     </row>
     <row r="47" spans="1:10">
@@ -2564,7 +2579,7 @@
         <v>56</v>
       </c>
       <c r="J48" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
     </row>
     <row r="49" spans="1:10">
@@ -2572,7 +2587,7 @@
         <v>57</v>
       </c>
       <c r="J49" t="s">
-        <v>264</v>
+        <v>279</v>
       </c>
     </row>
     <row r="50" spans="1:10">
@@ -2580,7 +2595,7 @@
         <v>58</v>
       </c>
       <c r="J50" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
     </row>
     <row r="51" spans="1:10">
@@ -2588,7 +2603,7 @@
         <v>59</v>
       </c>
       <c r="J51" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
     </row>
     <row r="52" spans="1:10">
@@ -2604,7 +2619,7 @@
         <v>61</v>
       </c>
       <c r="J53" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
     </row>
     <row r="54" spans="1:10">
@@ -2612,7 +2627,7 @@
         <v>62</v>
       </c>
       <c r="J54" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
     </row>
     <row r="55" spans="1:10">
@@ -2628,7 +2643,7 @@
         <v>64</v>
       </c>
       <c r="J56" t="s">
-        <v>264</v>
+        <v>282</v>
       </c>
     </row>
     <row r="57" spans="1:10">
@@ -2636,7 +2651,7 @@
         <v>65</v>
       </c>
       <c r="J57" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
     </row>
     <row r="58" spans="1:10">
@@ -2644,7 +2659,7 @@
         <v>66</v>
       </c>
       <c r="J58" t="s">
-        <v>264</v>
+        <v>284</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: Add Department and Status filters to Analytics Dashboard
- Add department dropdown filter to Analytics page
- Add status dropdown filter (pending/approved/rejected)
- Pass filters to backend API for filtered statistics
- Add Clear Filters button when filters are active
- Update tasks tracking spreadsheet (29/57 complete)

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/tasks_updated.xlsx
+++ b/tasks_updated.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="288">
   <si>
     <t>כותרת</t>
   </si>
@@ -799,7 +799,7 @@
     <t>✅ בוצע - כבר קיים useScrollToItem</t>
   </si>
   <si>
-    <t>⏳ לבדיקה - Export כבר מעביר פילטרים</t>
+    <t>✅ בוצע - הפרונטאנד כבר שולח את כל הפילטרים לייצוא, בעיה בבקאנד אם לא מכבד</t>
   </si>
   <si>
     <t>✅ בוצע - stopPropagation קיים</t>
@@ -820,6 +820,9 @@
     <t>⏳ לבדיקה</t>
   </si>
   <si>
+    <t>✅ בוצע - כפתור מחיקה כבר קיים למנג'רים ואדמינים</t>
+  </si>
+  <si>
     <t>✅ בוצע - כבר קיים בDepartmentManager</t>
   </si>
   <si>
@@ -829,6 +832,9 @@
     <t>✅ בוצע - נוסף מודל אישור</t>
   </si>
   <si>
+    <t>✅ בוצע - נוספו פילטרים של מחלקה וסטטוס ל-Analytics Dashboard</t>
+  </si>
+  <si>
     <t>✅ בוצע - נוסף quote_filename</t>
   </si>
   <si>
@@ -851,6 +857,9 @@
   </si>
   <si>
     <t>✅ בוצע - reset של input value</t>
+  </si>
+  <si>
+    <t>✅ בוצע - TomSelect תומך בהקלדה/חיפוש</t>
   </si>
   <si>
     <t>✅ בוצע - נוסף debounce + allowClear לדרופדאונים</t>
@@ -1586,7 +1595,7 @@
         <v>243</v>
       </c>
       <c r="J12" t="s">
-        <v>263</v>
+        <v>268</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -1644,7 +1653,7 @@
         <v>245</v>
       </c>
       <c r="J14" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -1673,7 +1682,7 @@
         <v>246</v>
       </c>
       <c r="J15" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -1702,7 +1711,7 @@
         <v>247</v>
       </c>
       <c r="J16" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -1731,7 +1740,7 @@
         <v>245</v>
       </c>
       <c r="J17" t="s">
-        <v>267</v>
+        <v>272</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -1789,7 +1798,7 @@
         <v>240</v>
       </c>
       <c r="J19" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -1818,7 +1827,7 @@
         <v>235</v>
       </c>
       <c r="J20" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -1847,7 +1856,7 @@
         <v>248</v>
       </c>
       <c r="J21" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -2027,7 +2036,7 @@
         <v>256</v>
       </c>
       <c r="J27" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -2056,7 +2065,7 @@
         <v>235</v>
       </c>
       <c r="J28" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -2114,7 +2123,7 @@
         <v>250</v>
       </c>
       <c r="J30" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -2172,7 +2181,7 @@
         <v>250</v>
       </c>
       <c r="J32" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
     </row>
     <row r="33" spans="1:10">
@@ -2410,7 +2419,7 @@
         <v>235</v>
       </c>
       <c r="J40" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
     </row>
     <row r="41" spans="1:10">
@@ -2563,7 +2572,7 @@
         <v>54</v>
       </c>
       <c r="J46" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
     </row>
     <row r="47" spans="1:10">
@@ -2579,7 +2588,7 @@
         <v>56</v>
       </c>
       <c r="J48" t="s">
-        <v>267</v>
+        <v>281</v>
       </c>
     </row>
     <row r="49" spans="1:10">
@@ -2587,7 +2596,7 @@
         <v>57</v>
       </c>
       <c r="J49" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
     </row>
     <row r="50" spans="1:10">
@@ -2619,7 +2628,7 @@
         <v>61</v>
       </c>
       <c r="J53" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
     </row>
     <row r="54" spans="1:10">
@@ -2627,7 +2636,7 @@
         <v>62</v>
       </c>
       <c r="J54" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
     </row>
     <row r="55" spans="1:10">
@@ -2643,7 +2652,7 @@
         <v>64</v>
       </c>
       <c r="J56" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
     </row>
     <row r="57" spans="1:10">
@@ -2651,7 +2660,7 @@
         <v>65</v>
       </c>
       <c r="J57" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
     </row>
     <row r="58" spans="1:10">
@@ -2659,7 +2668,7 @@
         <v>66</v>
       </c>
       <c r="J58" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: Improve expense details layout and search placeholders
- Add Department and Budget Year fields to ExpenseDetails
- Update search placeholders to show all searchable fields
- Update task tracking spreadsheet

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/tasks_updated.xlsx
+++ b/tasks_updated.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="293">
   <si>
     <t>כותרת</t>
   </si>
@@ -817,33 +817,39 @@
     <t>✅ בוצע - אין כפילות בקוד</t>
   </si>
   <si>
+    <t>✅ בוצע - שדה Date שופר ל-Document Date עם הסבר בעברית</t>
+  </si>
+  <si>
+    <t>✅ בוצע - כפתור מחיקה כבר קיים למנג'רים ואדמינים</t>
+  </si>
+  <si>
+    <t>✅ בוצע - נוספו שדות מחלקה ושנת תקציב לפירוט ההוצאה</t>
+  </si>
+  <si>
+    <t>✅ בוצע - כבר קיים בDepartmentManager</t>
+  </si>
+  <si>
+    <t>✅ בוצע - נוספו אייקונים וסטיילינג</t>
+  </si>
+  <si>
+    <t>✅ בוצע - נוסף מודל אישור</t>
+  </si>
+  <si>
+    <t>✅ בוצע - נוספו פילטרים של מחלקה וסטטוס ל-Analytics Dashboard</t>
+  </si>
+  <si>
+    <t>✅ בוצע - נוסף quote_filename</t>
+  </si>
+  <si>
+    <t>✅ בוצע - נוספו תוויות לקבצים</t>
+  </si>
+  <si>
+    <t>✅ בוצע - הטאב מוסתר בSidebar</t>
+  </si>
+  <si>
     <t>⏳ לבדיקה</t>
   </si>
   <si>
-    <t>✅ בוצע - כפתור מחיקה כבר קיים למנג'רים ואדמינים</t>
-  </si>
-  <si>
-    <t>✅ בוצע - כבר קיים בDepartmentManager</t>
-  </si>
-  <si>
-    <t>✅ בוצע - נוספו אייקונים וסטיילינג</t>
-  </si>
-  <si>
-    <t>✅ בוצע - נוסף מודל אישור</t>
-  </si>
-  <si>
-    <t>✅ בוצע - נוספו פילטרים של מחלקה וסטטוס ל-Analytics Dashboard</t>
-  </si>
-  <si>
-    <t>✅ בוצע - נוסף quote_filename</t>
-  </si>
-  <si>
-    <t>✅ בוצע - נוספו תוויות לקבצים</t>
-  </si>
-  <si>
-    <t>✅ בוצע - הטאב מוסתר בSidebar</t>
-  </si>
-  <si>
     <t>✅ בוצע - טבלאות ברוחב מלא</t>
   </si>
   <si>
@@ -853,6 +859,9 @@
     <t>✅ בוצע - נוסף debounce לפילטרים</t>
   </si>
   <si>
+    <t>✅ בוצע - שיפור placeholders בחיפוש להראות אילו שדות מחפשים, התנהגות תלויה בbackend</t>
+  </si>
+  <si>
     <t>✅ בוצע - כותרת sticky</t>
   </si>
   <si>
@@ -863,6 +872,12 @@
   </si>
   <si>
     <t>✅ בוצע - נוסף debounce + allowClear לדרופדאונים</t>
+  </si>
+  <si>
+    <t>⏳ לבדיקה - תלוי בbackend (ייצוא CSV צד שרת)</t>
+  </si>
+  <si>
+    <t>⏳ לבדיקה - תלוי בbackend (הפרונטאנד כבר יש לו pagination ו-debounce)</t>
   </si>
   <si>
     <t>✅ בוצע - Payment Due מותנה בbank_transfer</t>
@@ -1624,7 +1639,7 @@
         <v>244</v>
       </c>
       <c r="J13" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -1653,7 +1668,7 @@
         <v>245</v>
       </c>
       <c r="J14" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -1682,7 +1697,7 @@
         <v>246</v>
       </c>
       <c r="J15" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -1711,7 +1726,7 @@
         <v>247</v>
       </c>
       <c r="J16" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -1740,7 +1755,7 @@
         <v>245</v>
       </c>
       <c r="J17" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -1798,7 +1813,7 @@
         <v>240</v>
       </c>
       <c r="J19" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -1827,7 +1842,7 @@
         <v>235</v>
       </c>
       <c r="J20" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -1856,7 +1871,7 @@
         <v>248</v>
       </c>
       <c r="J21" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -1885,7 +1900,7 @@
         <v>249</v>
       </c>
       <c r="J22" t="s">
-        <v>267</v>
+        <v>277</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -1943,7 +1958,7 @@
         <v>249</v>
       </c>
       <c r="J24" t="s">
-        <v>267</v>
+        <v>277</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -2036,7 +2051,7 @@
         <v>256</v>
       </c>
       <c r="J27" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -2065,7 +2080,7 @@
         <v>235</v>
       </c>
       <c r="J28" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -2094,7 +2109,7 @@
         <v>249</v>
       </c>
       <c r="J29" t="s">
-        <v>267</v>
+        <v>277</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -2123,7 +2138,7 @@
         <v>250</v>
       </c>
       <c r="J30" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -2181,7 +2196,7 @@
         <v>250</v>
       </c>
       <c r="J32" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
     </row>
     <row r="33" spans="1:10">
@@ -2213,7 +2228,7 @@
         <v>257</v>
       </c>
       <c r="J33" t="s">
-        <v>267</v>
+        <v>277</v>
       </c>
     </row>
     <row r="34" spans="1:10">
@@ -2274,7 +2289,7 @@
         <v>250</v>
       </c>
       <c r="J35" t="s">
-        <v>267</v>
+        <v>281</v>
       </c>
     </row>
     <row r="36" spans="1:10">
@@ -2361,7 +2376,7 @@
         <v>235</v>
       </c>
       <c r="J38" t="s">
-        <v>267</v>
+        <v>277</v>
       </c>
     </row>
     <row r="39" spans="1:10">
@@ -2390,7 +2405,7 @@
         <v>240</v>
       </c>
       <c r="J39" t="s">
-        <v>267</v>
+        <v>277</v>
       </c>
     </row>
     <row r="40" spans="1:10">
@@ -2419,7 +2434,7 @@
         <v>235</v>
       </c>
       <c r="J40" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
     </row>
     <row r="41" spans="1:10">
@@ -2448,7 +2463,7 @@
         <v>250</v>
       </c>
       <c r="J41" t="s">
-        <v>267</v>
+        <v>277</v>
       </c>
     </row>
     <row r="42" spans="1:10">
@@ -2477,7 +2492,7 @@
         <v>250</v>
       </c>
       <c r="J42" t="s">
-        <v>267</v>
+        <v>277</v>
       </c>
     </row>
     <row r="43" spans="1:10">
@@ -2535,7 +2550,7 @@
         <v>250</v>
       </c>
       <c r="J44" t="s">
-        <v>267</v>
+        <v>277</v>
       </c>
     </row>
     <row r="45" spans="1:10">
@@ -2564,7 +2579,7 @@
         <v>235</v>
       </c>
       <c r="J45" t="s">
-        <v>267</v>
+        <v>277</v>
       </c>
     </row>
     <row r="46" spans="1:10">
@@ -2572,7 +2587,7 @@
         <v>54</v>
       </c>
       <c r="J46" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
     </row>
     <row r="47" spans="1:10">
@@ -2588,7 +2603,7 @@
         <v>56</v>
       </c>
       <c r="J48" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
     </row>
     <row r="49" spans="1:10">
@@ -2596,7 +2611,7 @@
         <v>57</v>
       </c>
       <c r="J49" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
     </row>
     <row r="50" spans="1:10">
@@ -2604,7 +2619,7 @@
         <v>58</v>
       </c>
       <c r="J50" t="s">
-        <v>267</v>
+        <v>286</v>
       </c>
     </row>
     <row r="51" spans="1:10">
@@ -2612,7 +2627,7 @@
         <v>59</v>
       </c>
       <c r="J51" t="s">
-        <v>267</v>
+        <v>287</v>
       </c>
     </row>
     <row r="52" spans="1:10">
@@ -2628,7 +2643,7 @@
         <v>61</v>
       </c>
       <c r="J53" t="s">
-        <v>283</v>
+        <v>288</v>
       </c>
     </row>
     <row r="54" spans="1:10">
@@ -2636,7 +2651,7 @@
         <v>62</v>
       </c>
       <c r="J54" t="s">
-        <v>284</v>
+        <v>289</v>
       </c>
     </row>
     <row r="55" spans="1:10">
@@ -2652,7 +2667,7 @@
         <v>64</v>
       </c>
       <c r="J56" t="s">
-        <v>285</v>
+        <v>290</v>
       </c>
     </row>
     <row r="57" spans="1:10">
@@ -2660,7 +2675,7 @@
         <v>65</v>
       </c>
       <c r="J57" t="s">
-        <v>286</v>
+        <v>291</v>
       </c>
     </row>
     <row r="58" spans="1:10">
@@ -2668,7 +2683,7 @@
         <v>66</v>
       </c>
       <c r="J58" t="s">
-        <v>287</v>
+        <v>292</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: Preserve ExpenseHistory filters in URL for back navigation
Filters are now synced to URL params so they persist when navigating
to expense details and back. This fixes the state loss issue (Task 6).

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/tasks_updated.xlsx
+++ b/tasks_updated.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="298">
   <si>
     <t>כותרת</t>
   </si>
@@ -808,6 +808,9 @@
     <t>⏳ לבדיקה - תלוי בbackend</t>
   </si>
   <si>
+    <t>✅ בוצע - פילטרים נשמרים ב-URL ונשמרים בניווט הלוך/חזור</t>
+  </si>
+  <si>
     <t>✅ בוצע - החיפוש כבר ריאקטיבי עם debounce</t>
   </si>
   <si>
@@ -847,7 +850,10 @@
     <t>✅ בוצע - הטאב מוסתר בSidebar</t>
   </si>
   <si>
-    <t>⏳ לבדיקה</t>
+    <t>⏳ מחכה להחלטת מוצר - צריך להגדיר היקף דוחות למנג׳ר</t>
+  </si>
+  <si>
+    <t>⏳ מחכה להחלטת מוצר - צריך להגדיר שדות חובה בטופס</t>
   </si>
   <si>
     <t>✅ בוצע - טבלאות ברוחב מלא</t>
@@ -856,10 +862,19 @@
     <t>✅ בוצע - TomSelectInput בעריכה</t>
   </si>
   <si>
+    <t>⏳ מחכה להחלטת מוצר - האם להוסיף שנת תקציב לתתי קטגוריות</t>
+  </si>
+  <si>
     <t>✅ בוצע - נוסף debounce לפילטרים</t>
   </si>
   <si>
+    <t>⏳ מחכה להחלטת מוצר - צריך להגדיר כללים להמרת מטבעות</t>
+  </si>
+  <si>
     <t>✅ בוצע - שיפור placeholders בחיפוש להראות אילו שדות מחפשים, התנהגות תלויה בbackend</t>
+  </si>
+  <si>
+    <t>N/A - טבלת הנחש היא מערכת חיצונית לא בקוד הזה</t>
   </si>
   <si>
     <t>✅ בוצע - כותרת sticky</t>
@@ -1462,7 +1477,7 @@
         <v>253</v>
       </c>
       <c r="J7" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -1491,7 +1506,7 @@
         <v>235</v>
       </c>
       <c r="J8" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -1520,7 +1535,7 @@
         <v>240</v>
       </c>
       <c r="J9" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -1549,7 +1564,7 @@
         <v>241</v>
       </c>
       <c r="J10" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -1581,7 +1596,7 @@
         <v>254</v>
       </c>
       <c r="J11" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -1610,7 +1625,7 @@
         <v>243</v>
       </c>
       <c r="J12" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -1639,7 +1654,7 @@
         <v>244</v>
       </c>
       <c r="J13" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -1668,7 +1683,7 @@
         <v>245</v>
       </c>
       <c r="J14" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -1697,7 +1712,7 @@
         <v>246</v>
       </c>
       <c r="J15" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -1726,7 +1741,7 @@
         <v>247</v>
       </c>
       <c r="J16" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -1755,7 +1770,7 @@
         <v>245</v>
       </c>
       <c r="J17" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -1813,7 +1828,7 @@
         <v>240</v>
       </c>
       <c r="J19" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -1842,7 +1857,7 @@
         <v>235</v>
       </c>
       <c r="J20" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -1871,7 +1886,7 @@
         <v>248</v>
       </c>
       <c r="J21" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -1900,7 +1915,7 @@
         <v>249</v>
       </c>
       <c r="J22" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -1958,7 +1973,7 @@
         <v>249</v>
       </c>
       <c r="J24" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -2051,7 +2066,7 @@
         <v>256</v>
       </c>
       <c r="J27" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -2080,7 +2095,7 @@
         <v>235</v>
       </c>
       <c r="J28" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -2109,7 +2124,7 @@
         <v>249</v>
       </c>
       <c r="J29" t="s">
-        <v>277</v>
+        <v>282</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -2138,7 +2153,7 @@
         <v>250</v>
       </c>
       <c r="J30" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -2196,7 +2211,7 @@
         <v>250</v>
       </c>
       <c r="J32" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
     </row>
     <row r="33" spans="1:10">
@@ -2228,7 +2243,7 @@
         <v>257</v>
       </c>
       <c r="J33" t="s">
-        <v>277</v>
+        <v>284</v>
       </c>
     </row>
     <row r="34" spans="1:10">
@@ -2289,7 +2304,7 @@
         <v>250</v>
       </c>
       <c r="J35" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
     </row>
     <row r="36" spans="1:10">
@@ -2376,7 +2391,7 @@
         <v>235</v>
       </c>
       <c r="J38" t="s">
-        <v>277</v>
+        <v>286</v>
       </c>
     </row>
     <row r="39" spans="1:10">
@@ -2405,7 +2420,7 @@
         <v>240</v>
       </c>
       <c r="J39" t="s">
-        <v>277</v>
+        <v>286</v>
       </c>
     </row>
     <row r="40" spans="1:10">
@@ -2434,7 +2449,7 @@
         <v>235</v>
       </c>
       <c r="J40" t="s">
-        <v>282</v>
+        <v>287</v>
       </c>
     </row>
     <row r="41" spans="1:10">
@@ -2463,7 +2478,7 @@
         <v>250</v>
       </c>
       <c r="J41" t="s">
-        <v>277</v>
+        <v>286</v>
       </c>
     </row>
     <row r="42" spans="1:10">
@@ -2492,7 +2507,7 @@
         <v>250</v>
       </c>
       <c r="J42" t="s">
-        <v>277</v>
+        <v>286</v>
       </c>
     </row>
     <row r="43" spans="1:10">
@@ -2521,7 +2536,7 @@
         <v>240</v>
       </c>
       <c r="J43" t="s">
-        <v>263</v>
+        <v>286</v>
       </c>
     </row>
     <row r="44" spans="1:10">
@@ -2550,7 +2565,7 @@
         <v>250</v>
       </c>
       <c r="J44" t="s">
-        <v>277</v>
+        <v>286</v>
       </c>
     </row>
     <row r="45" spans="1:10">
@@ -2579,7 +2594,7 @@
         <v>235</v>
       </c>
       <c r="J45" t="s">
-        <v>277</v>
+        <v>286</v>
       </c>
     </row>
     <row r="46" spans="1:10">
@@ -2587,7 +2602,7 @@
         <v>54</v>
       </c>
       <c r="J46" t="s">
-        <v>283</v>
+        <v>288</v>
       </c>
     </row>
     <row r="47" spans="1:10">
@@ -2595,7 +2610,7 @@
         <v>55</v>
       </c>
       <c r="J47" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="48" spans="1:10">
@@ -2603,7 +2618,7 @@
         <v>56</v>
       </c>
       <c r="J48" t="s">
-        <v>284</v>
+        <v>289</v>
       </c>
     </row>
     <row r="49" spans="1:10">
@@ -2611,7 +2626,7 @@
         <v>57</v>
       </c>
       <c r="J49" t="s">
-        <v>285</v>
+        <v>290</v>
       </c>
     </row>
     <row r="50" spans="1:10">
@@ -2619,7 +2634,7 @@
         <v>58</v>
       </c>
       <c r="J50" t="s">
-        <v>286</v>
+        <v>291</v>
       </c>
     </row>
     <row r="51" spans="1:10">
@@ -2627,7 +2642,7 @@
         <v>59</v>
       </c>
       <c r="J51" t="s">
-        <v>287</v>
+        <v>292</v>
       </c>
     </row>
     <row r="52" spans="1:10">
@@ -2643,7 +2658,7 @@
         <v>61</v>
       </c>
       <c r="J53" t="s">
-        <v>288</v>
+        <v>293</v>
       </c>
     </row>
     <row r="54" spans="1:10">
@@ -2651,7 +2666,7 @@
         <v>62</v>
       </c>
       <c r="J54" t="s">
-        <v>289</v>
+        <v>294</v>
       </c>
     </row>
     <row r="55" spans="1:10">
@@ -2667,7 +2682,7 @@
         <v>64</v>
       </c>
       <c r="J56" t="s">
-        <v>290</v>
+        <v>295</v>
       </c>
     </row>
     <row r="57" spans="1:10">
@@ -2675,7 +2690,7 @@
         <v>65</v>
       </c>
       <c r="J57" t="s">
-        <v>291</v>
+        <v>296</v>
       </c>
     </row>
     <row r="58" spans="1:10">
@@ -2683,7 +2698,7 @@
         <v>66</v>
       </c>
       <c r="J58" t="s">
-        <v>292</v>
+        <v>297</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: Refresh user session after editing own profile in UserManagement
When an admin edits their own user record, the app now refreshes their
session to immediately reflect role/permission changes (Task 17 partial fix).

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/tasks_updated.xlsx
+++ b/tasks_updated.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="300">
   <si>
     <t>כותרת</t>
   </si>
@@ -841,6 +841,9 @@
     <t>✅ בוצע - נוספו פילטרים של מחלקה וסטטוס ל-Analytics Dashboard</t>
   </si>
   <si>
+    <t>✅ בוצע חלקית - הפרונטאנד מרענן את ה-user state אם האדמין עורך את עצמו, עדיין תלוי בbackend לעדכון משתמשים אחרים</t>
+  </si>
+  <si>
     <t>✅ בוצע - נוסף quote_filename</t>
   </si>
   <si>
@@ -899,6 +902,9 @@
   </si>
   <si>
     <t>✅ בוצע - לחיצה על שורה פותחת פרטים</t>
+  </si>
+  <si>
+    <t>✅ בוצע - טאב Approvals הוסתר, דרופדאון expense type הוסתר, כל הוצאה מוגשת כ-auto_approved</t>
   </si>
   <si>
     <t>✅ בוצע - כבר קיים TomSelect עם createNewOption</t>
@@ -1799,7 +1805,7 @@
         <v>239</v>
       </c>
       <c r="J18" t="s">
-        <v>263</v>
+        <v>275</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -1828,7 +1834,7 @@
         <v>240</v>
       </c>
       <c r="J19" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -1857,7 +1863,7 @@
         <v>235</v>
       </c>
       <c r="J20" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -1886,7 +1892,7 @@
         <v>248</v>
       </c>
       <c r="J21" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -1915,7 +1921,7 @@
         <v>249</v>
       </c>
       <c r="J22" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -1973,7 +1979,7 @@
         <v>249</v>
       </c>
       <c r="J24" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -2066,7 +2072,7 @@
         <v>256</v>
       </c>
       <c r="J27" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -2095,7 +2101,7 @@
         <v>235</v>
       </c>
       <c r="J28" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -2124,7 +2130,7 @@
         <v>249</v>
       </c>
       <c r="J29" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -2153,7 +2159,7 @@
         <v>250</v>
       </c>
       <c r="J30" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -2211,7 +2217,7 @@
         <v>250</v>
       </c>
       <c r="J32" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="33" spans="1:10">
@@ -2243,7 +2249,7 @@
         <v>257</v>
       </c>
       <c r="J33" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="34" spans="1:10">
@@ -2304,7 +2310,7 @@
         <v>250</v>
       </c>
       <c r="J35" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="36" spans="1:10">
@@ -2391,7 +2397,7 @@
         <v>235</v>
       </c>
       <c r="J38" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="39" spans="1:10">
@@ -2420,7 +2426,7 @@
         <v>240</v>
       </c>
       <c r="J39" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="40" spans="1:10">
@@ -2449,7 +2455,7 @@
         <v>235</v>
       </c>
       <c r="J40" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="41" spans="1:10">
@@ -2478,7 +2484,7 @@
         <v>250</v>
       </c>
       <c r="J41" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="42" spans="1:10">
@@ -2507,7 +2513,7 @@
         <v>250</v>
       </c>
       <c r="J42" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="43" spans="1:10">
@@ -2536,7 +2542,7 @@
         <v>240</v>
       </c>
       <c r="J43" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="44" spans="1:10">
@@ -2565,7 +2571,7 @@
         <v>250</v>
       </c>
       <c r="J44" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="45" spans="1:10">
@@ -2594,7 +2600,7 @@
         <v>235</v>
       </c>
       <c r="J45" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="46" spans="1:10">
@@ -2602,7 +2608,7 @@
         <v>54</v>
       </c>
       <c r="J46" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="47" spans="1:10">
@@ -2618,7 +2624,7 @@
         <v>56</v>
       </c>
       <c r="J48" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
     </row>
     <row r="49" spans="1:10">
@@ -2626,7 +2632,7 @@
         <v>57</v>
       </c>
       <c r="J49" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
     </row>
     <row r="50" spans="1:10">
@@ -2634,7 +2640,7 @@
         <v>58</v>
       </c>
       <c r="J50" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="51" spans="1:10">
@@ -2642,7 +2648,7 @@
         <v>59</v>
       </c>
       <c r="J51" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
     </row>
     <row r="52" spans="1:10">
@@ -2658,7 +2664,7 @@
         <v>61</v>
       </c>
       <c r="J53" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
     </row>
     <row r="54" spans="1:10">
@@ -2666,7 +2672,7 @@
         <v>62</v>
       </c>
       <c r="J54" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
     <row r="55" spans="1:10">
@@ -2674,7 +2680,7 @@
         <v>63</v>
       </c>
       <c r="J55" t="s">
-        <v>263</v>
+        <v>296</v>
       </c>
     </row>
     <row r="56" spans="1:10">
@@ -2682,7 +2688,7 @@
         <v>64</v>
       </c>
       <c r="J56" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
     </row>
     <row r="57" spans="1:10">
@@ -2690,7 +2696,7 @@
         <v>65</v>
       </c>
       <c r="J57" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
     </row>
     <row r="58" spans="1:10">
@@ -2698,7 +2704,7 @@
         <v>66</v>
       </c>
       <c r="J58" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
     </row>
   </sheetData>

</xml_diff>